<commit_message>
updated BOM with cost
</commit_message>
<xml_diff>
--- a/USB PD Trigger Board_XL_BOM.xlsx
+++ b/USB PD Trigger Board_XL_BOM.xlsx
@@ -8,13 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wajah\Documents\KiCad\9.0\projects\USB_PD_Trigger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65294D84-506B-4DC5-BE27-A771CE22E427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C590008C-EAA4-4863-841C-42D783ACFD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{09059CB2-B047-49BC-A9FC-7E5F3CE728EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$E$1:$E$29</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$I$34</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$E$2:$E$30</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$E$2:$H$30</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$E$30</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$H$34</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$I$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$I$2:$I$30</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$I$34</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$H$34</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="111">
   <si>
     <t>Ref Des</t>
   </si>
@@ -264,24 +279,9 @@
     <t>C1, C3, C9, C10</t>
   </si>
   <si>
-    <t>D4, D5</t>
-  </si>
-  <si>
-    <t>ESD441DPLR</t>
-  </si>
-  <si>
-    <t>ESD321DPYR</t>
-  </si>
-  <si>
-    <t>TVS DIODE 3.6VWM 6.8VC 2X1SON</t>
-  </si>
-  <si>
     <t>Texas Instruments</t>
   </si>
   <si>
-    <t>TVS DIODE 5.5VWM 7.6VC 2X2SON</t>
-  </si>
-  <si>
     <t>Qty</t>
   </si>
   <si>
@@ -348,13 +348,40 @@
     <t>Alternates/Substitutes</t>
   </si>
   <si>
-    <t>D5, D6</t>
+    <t>DT1452-02SO-7</t>
+  </si>
+  <si>
+    <t>TVS DIODE 5.5VWM 11VC SOT233</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>ESDS312DBVR</t>
+  </si>
+  <si>
+    <t>TVS DIODE 3.6VWM 6.5VC SOT23-5</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Shipping cost</t>
+  </si>
+  <si>
+    <t>Total cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -444,14 +471,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,6 +490,1420 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="19"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="20"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="21"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="22"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="23"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="24"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$2:$E$26</c:f>
+              <c:strCache>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>CL31B106KBHNNNE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GRM188R71H104KA93D</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CC0603KRX7R9BB105</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>CC0603KRX7R9BB103</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>APT2012CGCK</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>APT2012LVBC/D</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>APT2012SECK/J4-PRV</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DT1452-02SO-7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>ESDS312DBVR</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>AP33771CFBZ-13-FA01</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>HP8KB7TB1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>RC0603FR-07100KL</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>PA1206FRF7W0R005L</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>RC0603JR-076K2L</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>AF0603JR-07200RL</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>RC0603FR-0782KL</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>RC0603FR-0766K5L</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>RC0603FR-0752K3L</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>RC0603FR-0739KL</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>RC0603FR-0726K1L</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>RC0603FR-0715KL</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>RC0603FR-075K1L</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>RC0603JR-071KL</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>RC0603JR-070RL</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>PZ254V-12-16P</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>"₹"\ #,##0.00</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>271</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>834</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1850</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8802-4A90-9C3A-44603391745E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.78656269497336206"/>
+          <c:y val="2.4821939871152471E-2"/>
+          <c:w val="0.20699089084452679"/>
+          <c:h val="0.96757188021951801"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5DB7092-3C33-2C9D-C68D-4DC2281FD69E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -766,10 +2203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAFBAE5-7872-4769-9B4A-5A7E0BBFE69F}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,9 +2219,10 @@
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -792,7 +2230,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>4</v>
@@ -804,17 +2242,20 @@
         <v>2</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="11" t="s">
         <v>78</v>
       </c>
       <c r="C2" s="2">
@@ -831,12 +2272,15 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="13">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="11" t="s">
         <v>76</v>
       </c>
       <c r="C3" s="2">
@@ -853,12 +2297,15 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="13">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C4" s="2">
@@ -875,12 +2322,15 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="13">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="11" t="s">
         <v>75</v>
       </c>
       <c r="C5" s="2">
@@ -897,12 +2347,15 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2">
@@ -919,12 +2372,15 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="13">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="2">
@@ -941,12 +2397,15 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="13">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="11" t="s">
         <v>63</v>
       </c>
       <c r="C8" s="2">
@@ -963,56 +2422,65 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="13">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>79</v>
+      <c r="B9" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="C9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="13">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="2">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="13">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="2">
@@ -1029,12 +2497,15 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="13">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="2">
@@ -1051,12 +2522,15 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="13">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="2">
@@ -1073,12 +2547,15 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="2">
@@ -1095,12 +2572,15 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="13">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="2">
@@ -1117,12 +2597,15 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="13">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="2">
@@ -1139,12 +2622,15 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="13">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C17" s="2">
@@ -1161,12 +2647,15 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="11" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="2">
@@ -1183,12 +2672,15 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="2">
@@ -1205,12 +2697,15 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="2">
@@ -1227,12 +2722,15 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="2">
@@ -1249,12 +2747,15 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C22" s="2">
@@ -1271,12 +2772,15 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="11" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="2">
@@ -1293,12 +2797,15 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="2">
@@ -1315,12 +2822,15 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="13">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C25" s="2">
@@ -1337,118 +2847,128 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C26" s="2">
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>91</v>
+        <v>85</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="I26" s="13"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="13"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>26</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>103</v>
+        <v>27</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="C28" s="2">
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>104</v>
+        <v>96</v>
+      </c>
+      <c r="E28" s="7">
+        <v>2171790001</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="13">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E29" s="7">
-        <v>2171790001</v>
+        <v>95</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>27</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>95</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I29" s="13"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="1"/>
       <c r="G30" s="7" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="I30" s="13"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
@@ -1456,74 +2976,52 @@
       <c r="E31" s="7"/>
       <c r="F31" s="1"/>
       <c r="G31" s="9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="I31" s="13"/>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I33" s="13">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I34" s="13">
+        <f>SUM(I2:I33)</f>
+        <v>5838</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I1" xr:uid="{CEAFBAE5-7872-4769-9B4A-5A7E0BBFE69F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I31">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C43E65-CB09-481B-B8C5-633876E8C677}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC16" sqref="AC16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>